<commit_message>
minor updates to be more replicable to other systems
</commit_message>
<xml_diff>
--- a/input/input_parameters.xlsx
+++ b/input/input_parameters.xlsx
@@ -600,7 +600,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +657,7 @@
         <v>5000</v>
       </c>
       <c r="E2" s="5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F2" s="5">
         <v>15</v>
@@ -694,7 +694,7 @@
       </c>
       <c r="C11" s="6">
         <f>(($E$2*Distributions!$B$2*Distributions!$C$2+$E$2*Distributions!$B$3*(1-Distributions!$E$2)+$E$2*Distributions!B3*Distributions!E2*(1-Distributions!$F$2)+$E$2*Distributions!B4*(1-Distributions!$F$2))*7) + $E$2*7</f>
-        <v>533.03250000000003</v>
+        <v>106.6065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated "Estimating Return Demand" file
</commit_message>
<xml_diff>
--- a/input/input_parameters.xlsx
+++ b/input/input_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Parameters" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>Replications</t>
   </si>
@@ -175,9 +175,6 @@
     <t>Results</t>
   </si>
   <si>
-    <t>Visit</t>
-  </si>
-  <si>
     <t>Scan Result</t>
   </si>
 </sst>
@@ -239,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -371,27 +368,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left/>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -401,7 +383,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -439,12 +421,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -3299,11 +3291,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="168380928"/>
-        <c:axId val="69401344"/>
+        <c:axId val="281168384"/>
+        <c:axId val="153090816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="168380928"/>
+        <c:axId val="281168384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3312,7 +3304,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69401344"/>
+        <c:crossAx val="153090816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3320,7 +3312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69401344"/>
+        <c:axId val="153090816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3331,7 +3323,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168380928"/>
+        <c:crossAx val="281168384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3676,7 +3668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -3796,17 +3788,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
@@ -3814,20 +3806,20 @@
     <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="29">
+        <v>3</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="31" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -3837,29 +3829,29 @@
         <v>17</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="32">
         <v>1</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="33">
         <v>0.85</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="33">
         <v>0.13</v>
       </c>
-      <c r="E2" s="28">
+      <c r="E2" s="34">
         <v>0.02</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="18">
         <v>0.91</v>
       </c>
       <c r="G2" s="9">
@@ -3868,30 +3860,30 @@
       <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="28">
+      <c r="I2" s="26">
         <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="25">
         <v>0.47499999999999998</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="25">
         <v>0.29000000000000004</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="26">
         <v>0.23500000000000001</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="30">
+      <c r="I3" s="28">
         <v>0.85</v>
       </c>
       <c r="J3" t="s">
@@ -3899,19 +3891,19 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="27">
         <v>0.1</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="27">
         <v>0.45</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="28">
         <v>0.45</v>
       </c>
       <c r="F4" s="16"/>

</xml_diff>

<commit_message>
changed r script to use relative path
</commit_message>
<xml_diff>
--- a/input/input_parameters.xlsx
+++ b/input/input_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General Parameters" sheetId="1" r:id="rId1"/>
@@ -3291,11 +3291,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="211831296"/>
-        <c:axId val="155646720"/>
+        <c:axId val="231066112"/>
+        <c:axId val="119864064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="211831296"/>
+        <c:axId val="231066112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3304,7 +3304,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155646720"/>
+        <c:crossAx val="119864064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3312,7 +3312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="155646720"/>
+        <c:axId val="119864064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3323,14 +3323,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="211831296"/>
+        <c:crossAx val="231066112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3669,8 +3668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4254,8 +4253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
refactoring code to allow easier scenario testing
</commit_message>
<xml_diff>
--- a/input/input_parameters.xlsx
+++ b/input/input_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="General Parameters" sheetId="1" r:id="rId1"/>
@@ -3316,11 +3316,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="211827200"/>
-        <c:axId val="155056896"/>
+        <c:axId val="284441088"/>
+        <c:axId val="152828672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="211827200"/>
+        <c:axId val="284441088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3329,7 +3329,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155056896"/>
+        <c:crossAx val="152828672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3337,7 +3337,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="155056896"/>
+        <c:axId val="152828672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3348,7 +3348,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="211827200"/>
+        <c:crossAx val="284441088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3693,8 +3693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3742,18 +3742,16 @@
         <v>30</v>
       </c>
       <c r="B2" s="3">
-        <f>30*12*3</f>
-        <v>1080</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
-        <f>30*12*6</f>
-        <v>2160</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
       </c>
       <c r="E2" s="3">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
         <v>15</v>
@@ -3781,7 +3779,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4058,8 +4056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4086,7 +4084,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
-        <v>0</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="B3">
         <f>30*6</f>
@@ -4095,7 +4093,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
-        <v>1</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="B4">
         <f>30*3</f>
@@ -4140,8 +4138,8 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f>30*6</f>
-        <v>180</v>
+        <f>30*12</f>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -4154,7 +4152,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed cancer probability bug and updated results
-30 to 40 arrival rate is done
</commit_message>
<xml_diff>
--- a/input/input_parameters.xlsx
+++ b/input/input_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General Parameters" sheetId="1" r:id="rId1"/>
@@ -411,7 +411,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -462,6 +462,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -3316,11 +3319,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="284441088"/>
-        <c:axId val="152828672"/>
+        <c:axId val="282479104"/>
+        <c:axId val="134675200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="284441088"/>
+        <c:axId val="282479104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3329,7 +3332,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152828672"/>
+        <c:crossAx val="134675200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3337,7 +3340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152828672"/>
+        <c:axId val="134675200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3348,13 +3351,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="284441088"/>
+        <c:crossAx val="282479104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3693,8 +3697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3742,16 +3746,18 @@
         <v>30</v>
       </c>
       <c r="B2" s="3">
-        <v>0</v>
+        <f>30*12*3</f>
+        <v>1080</v>
       </c>
       <c r="C2" s="3">
-        <v>10</v>
+        <f>30*12*6</f>
+        <v>2160</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
       </c>
       <c r="E2" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F2" s="3">
         <v>15</v>
@@ -4149,10 +4155,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4162,7 +4168,7 @@
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
@@ -4176,7 +4182,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -4191,7 +4197,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -4202,7 +4208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -4213,7 +4219,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -4224,55 +4230,91 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -4287,7 +4329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
trying to fix bugs
</commit_message>
<xml_diff>
--- a/input/input_parameters.xlsx
+++ b/input/input_parameters.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
   <si>
     <t>Replications</t>
   </si>
@@ -38,15 +38,6 @@
   </si>
   <si>
     <t>Service Time (minutes)</t>
-  </si>
-  <si>
-    <t>Ottawa Hospital Scan Capacity</t>
-  </si>
-  <si>
-    <t>Renfew Scan Capacity</t>
-  </si>
-  <si>
-    <t>Cornwall Scan Capacity</t>
   </si>
   <si>
     <t>Negative</t>
@@ -74,9 +65,6 @@
   </si>
   <si>
     <t>Suspicious Result Needs Biopsy probability</t>
-  </si>
-  <si>
-    <t>Probability a person with negative result stays in the system</t>
   </si>
   <si>
     <t>Stage_1</t>
@@ -168,6 +156,12 @@
   <si>
     <t>Number of Negatives, to leave system</t>
   </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Probability a person with negative result leaves the system</t>
+  </si>
 </sst>
 </file>
 
@@ -227,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -325,28 +319,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -356,15 +328,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -411,7 +374,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -440,28 +403,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -3319,11 +3268,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="294714880"/>
-        <c:axId val="151256384"/>
+        <c:axId val="291616768"/>
+        <c:axId val="105716480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="294714880"/>
+        <c:axId val="291616768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3332,7 +3281,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151256384"/>
+        <c:crossAx val="105716480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3340,7 +3289,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151256384"/>
+        <c:axId val="105716480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3351,7 +3300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="294714880"/>
+        <c:crossAx val="291616768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3694,10 +3643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3711,7 +3660,7 @@
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3730,17 +3679,11 @@
       <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>30</v>
       </c>
@@ -3761,17 +3704,11 @@
       <c r="F2" s="3">
         <v>15</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>1</v>
       </c>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
-      <c r="I2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" s="13"/>
     </row>
   </sheetData>
@@ -3781,276 +3718,225 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="26">
-        <v>1</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="28" t="s">
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="32">
-        <v>1</v>
-      </c>
-      <c r="C2" s="30">
+      <c r="G1" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="25">
         <v>0.85</v>
       </c>
-      <c r="D2" s="30">
+      <c r="C2" s="16">
+        <v>0.09</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0.62</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="G2" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="26">
         <v>0.13</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="24">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="27">
         <v>0.02</v>
       </c>
-      <c r="F2" s="16">
-        <v>0.91</v>
-      </c>
-      <c r="G2" s="9">
-        <v>0.62</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="24">
-        <v>0.75</v>
-      </c>
-      <c r="J2" s="35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="H3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="25">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="20"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J6" s="14"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I7" s="14"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I8" s="14"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E12" s="14"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-    </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="14"/>
+      <c r="D4" s="20"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="14"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="21"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E18" s="10"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-    </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-    </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-    </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-    </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-    </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-    </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-    </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-    </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-    </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-    </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-    </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-    </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4062,7 +3948,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4075,16 +3961,16 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4126,16 +4012,16 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4157,7 +4043,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4169,21 +4055,21 @@
   <sheetData>
     <row r="1" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" s="8">
         <v>0.63</v>
@@ -4198,7 +4084,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B3" s="8">
         <v>7.0000000000000007E-2</v>
@@ -4209,7 +4095,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" s="8">
         <v>0.15</v>
@@ -4220,7 +4106,7 @@
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B5" s="16">
         <v>0.15</v>
@@ -4236,7 +4122,7 @@
       <c r="B8" s="14"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -4248,10 +4134,10 @@
       <c r="T12" s="20"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -4260,10 +4146,10 @@
       <c r="T13" s="20"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
       <c r="E14" s="20"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -4273,9 +4159,9 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
       <c r="E15" s="20"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -4285,9 +4171,9 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
       <c r="E16" s="20"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -4297,9 +4183,9 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
       <c r="E17" s="20"/>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -4328,7 +4214,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4338,55 +4226,55 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>24</v>
@@ -4394,7 +4282,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>24</v>
@@ -4424,43 +4312,43 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="J1" s="12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="P1" s="17" t="s">
-        <v>38</v>
       </c>
       <c r="Q1" s="12"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" s="18">
         <v>0.63</v>
@@ -4469,10 +4357,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J2" s="18">
         <f>B2</f>
@@ -4499,7 +4387,7 @@
         <v>0.3</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="R2" s="10">
         <f>J2+$C$2</f>
@@ -4524,7 +4412,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" s="18">
         <v>7.0000000000000007E-2</v>
@@ -4586,7 +4474,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B4" s="18">
         <v>0.15</v>
@@ -4648,7 +4536,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" s="18">
         <v>0.15</v>
@@ -4816,22 +4704,22 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="I8" s="12">
         <v>6</v>
@@ -4887,7 +4775,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B9" s="18">
         <v>0.63</v>

</xml_diff>